<commit_message>
FY18, 19 & 20 data entry
</commit_message>
<xml_diff>
--- a/$AXON.xlsx
+++ b/$AXON.xlsx
@@ -1,25 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB67E4B-1BC3-407F-912E-03DE6D34E469}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54A9C6A-8C08-7747-ABA7-D33D73713413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{309C4E68-998D-4D03-B9D9-E68F5F237DED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{309C4E68-998D-4D03-B9D9-E68F5F237DED}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Financial Model" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Financial Model'!$U$5:$AI$5</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'Financial Model'!$U$5:$AI$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -135,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="176">
   <si>
     <t>$AXON</t>
   </si>
@@ -605,9 +619,6 @@
     <t>Q419</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>US Secret Service</t>
   </si>
   <si>
@@ -663,17 +674,19 @@
   </si>
   <si>
     <t>Upside</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0\x"/>
-    <numFmt numFmtId="173" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -919,7 +932,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1024,43 +1037,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1082,15 +1058,57 @@
     <xf numFmtId="166" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1582,57 +1600,57 @@
   <dimension ref="A2:AA37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="C28" sqref="C28:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B5" s="62" t="s">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="B5" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="64"/>
-      <c r="G5" s="62" t="s">
+      <c r="C5" s="78"/>
+      <c r="D5" s="79"/>
+      <c r="G5" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="64"/>
-      <c r="R5" s="62" t="s">
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="79"/>
+      <c r="R5" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="63"/>
-      <c r="T5" s="63"/>
-      <c r="U5" s="64"/>
-      <c r="X5" s="62" t="s">
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
+      <c r="U5" s="79"/>
+      <c r="X5" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="Y5" s="63"/>
-      <c r="Z5" s="63"/>
-      <c r="AA5" s="64"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Y5" s="78"/>
+      <c r="Z5" s="78"/>
+      <c r="AA5" s="79"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1657,13 +1675,13 @@
       <c r="T6" s="25"/>
       <c r="U6" s="26"/>
       <c r="X6" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="13"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1691,13 +1709,13 @@
       <c r="T7" s="25"/>
       <c r="U7" s="26"/>
       <c r="X7" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
       <c r="AA7" s="13"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1727,7 +1745,7 @@
       <c r="Z8" s="12"/>
       <c r="AA8" s="13"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1759,7 +1777,7 @@
       <c r="Z9" s="12"/>
       <c r="AA9" s="13"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1795,7 +1813,7 @@
       <c r="Z10" s="14"/>
       <c r="AA10" s="15"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1823,7 +1841,7 @@
       <c r="T11" s="8"/>
       <c r="U11" s="9"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
@@ -1849,7 +1867,7 @@
       <c r="T12" s="8"/>
       <c r="U12" s="9"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
       <c r="G13" s="18"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -1867,7 +1885,7 @@
       <c r="T13" s="8"/>
       <c r="U13" s="9"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
       <c r="G14" s="18"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -1885,12 +1903,12 @@
       <c r="T14" s="8"/>
       <c r="U14" s="9"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B15" s="62" t="s">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="B15" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="64"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="79"/>
       <c r="G15" s="18"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -1908,17 +1926,17 @@
       <c r="T15" s="8"/>
       <c r="U15" s="9"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A16" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="71" t="s">
+      <c r="C16" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="72"/>
+      <c r="D16" s="83"/>
       <c r="G16" s="18"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -1936,17 +1954,17 @@
       <c r="T16" s="8"/>
       <c r="U16" s="9"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="71" t="s">
+      <c r="C17" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="72"/>
+      <c r="D17" s="83"/>
       <c r="G17" s="18"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -1964,14 +1982,14 @@
       <c r="T17" s="8"/>
       <c r="U17" s="9"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="72"/>
+      <c r="D18" s="83"/>
       <c r="G18" s="18"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -1987,14 +2005,14 @@
       <c r="T18" s="8"/>
       <c r="U18" s="9"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B19" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="74"/>
+      <c r="D19" s="85"/>
       <c r="G19" s="18"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
@@ -2012,7 +2030,7 @@
       <c r="T19" s="8"/>
       <c r="U19" s="9"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="G20" s="18"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
@@ -2030,7 +2048,7 @@
       <c r="T20" s="8"/>
       <c r="U20" s="9"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="G21" s="18"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
@@ -2048,12 +2066,12 @@
       <c r="T21" s="8"/>
       <c r="U21" s="9"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B22" s="62" t="s">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="B22" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="64"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="79"/>
       <c r="G22" s="18"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
@@ -2069,14 +2087,14 @@
       <c r="T22" s="8"/>
       <c r="U22" s="9"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B23" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="72"/>
+      <c r="D23" s="83"/>
       <c r="G23" s="18"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -2094,14 +2112,14 @@
       <c r="T23" s="8"/>
       <c r="U23" s="9"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B24" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="71">
+      <c r="C24" s="82">
         <v>1993</v>
       </c>
-      <c r="D24" s="72"/>
+      <c r="D24" s="83"/>
       <c r="G24" s="18"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -2119,10 +2137,10 @@
       <c r="T24" s="8"/>
       <c r="U24" s="9"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B25" s="18"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="70"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81"/>
       <c r="G25" s="54">
         <v>43221</v>
       </c>
@@ -2144,10 +2162,10 @@
       <c r="T25" s="8"/>
       <c r="U25" s="9"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B26" s="18"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="70"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
       <c r="G26" s="18"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
@@ -2163,7 +2181,7 @@
       <c r="T26" s="8"/>
       <c r="U26" s="9"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B27" s="18" t="s">
         <v>19</v>
       </c>
@@ -2188,14 +2206,14 @@
       <c r="T27" s="8"/>
       <c r="U27" s="9"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B28" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="60" t="s">
-        <v>156</v>
-      </c>
-      <c r="D28" s="61"/>
+      <c r="C28" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="D28" s="87"/>
       <c r="G28" s="19">
         <v>2007</v>
       </c>
@@ -2217,7 +2235,7 @@
       <c r="T28" s="8"/>
       <c r="U28" s="9"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="R29" s="31" t="s">
         <v>51</v>
       </c>
@@ -2225,66 +2243,71 @@
       <c r="T29" s="10"/>
       <c r="U29" s="11"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B31" s="62" t="s">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="B31" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="63"/>
-      <c r="D31" s="64"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C31" s="78"/>
+      <c r="D31" s="79"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B32" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="65">
+      <c r="C32" s="88">
         <f>C8/SUM('Financial Model'!N5:Q5)</f>
         <v>12.532665911248298</v>
       </c>
-      <c r="D32" s="66"/>
+      <c r="D32" s="89"/>
       <c r="R32" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B33" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="65">
+      <c r="C33" s="88">
         <f>C6/'Financial Model'!Q84</f>
         <v>10.904968309556024</v>
       </c>
-      <c r="D33" s="66"/>
+      <c r="D33" s="89"/>
       <c r="R33" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B34" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="67"/>
-      <c r="D34" s="68"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="91"/>
       <c r="R34" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.15">
       <c r="R35" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.15">
       <c r="R36" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.15">
       <c r="R37" s="1" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="R5:U5"/>
     <mergeCell ref="X5:AA5"/>
@@ -2299,11 +2322,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C28:D28" r:id="rId1" display="Link" xr:uid="{79BCDA43-1DBD-4865-999E-0DD05314FB66}"/>
@@ -2320,27 +2338,28 @@
   <dimension ref="A1:BU99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W10" sqref="V10:W10"/>
+      <selection pane="bottomRight" activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="9.140625" style="80"/>
-    <col min="18" max="18" width="9.140625" style="48"/>
-    <col min="19" max="24" width="9.140625" style="1"/>
-    <col min="25" max="25" width="9.140625" style="48"/>
-    <col min="26" max="37" width="9.140625" style="1"/>
-    <col min="38" max="38" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="16" width="9.1640625" style="1"/>
+    <col min="17" max="17" width="9.1640625" style="65"/>
+    <col min="18" max="18" width="9.1640625" style="48"/>
+    <col min="19" max="24" width="9.1640625" style="1"/>
+    <col min="25" max="25" width="9.1640625" style="48"/>
+    <col min="26" max="36" width="9.1640625" style="1"/>
+    <col min="37" max="37" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:35" s="34" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C1" s="34" t="s">
         <v>152</v>
       </c>
@@ -2383,10 +2402,10 @@
       <c r="P1" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="76" t="s">
+      <c r="Q1" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="84" t="s">
+      <c r="R1" s="69" t="s">
         <v>97</v>
       </c>
       <c r="U1" s="34" t="s">
@@ -2395,47 +2414,47 @@
       <c r="V1" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="W1" s="49" t="s">
         <v>86</v>
       </c>
       <c r="X1" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="Y1" s="84" t="s">
+      <c r="Y1" s="69" t="s">
         <v>88</v>
       </c>
       <c r="Z1" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA1" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="AA1" s="34" t="s">
+      <c r="AB1" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="AB1" s="34" t="s">
+      <c r="AC1" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="AC1" s="34" t="s">
+      <c r="AD1" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="AD1" s="34" t="s">
+      <c r="AE1" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="AE1" s="34" t="s">
+      <c r="AF1" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="AF1" s="34" t="s">
+      <c r="AG1" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="AG1" s="34" t="s">
+      <c r="AH1" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="AH1" s="34" t="s">
+      <c r="AI1" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="AI1" s="34" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="2:35" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="2:35" s="32" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B2" s="33"/>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
@@ -2465,12 +2484,21 @@
       <c r="P2" s="37">
         <v>44742</v>
       </c>
-      <c r="Q2" s="82">
+      <c r="Q2" s="67">
         <v>44834</v>
       </c>
       <c r="R2" s="46" t="s">
         <v>58</v>
       </c>
+      <c r="U2" s="37">
+        <v>43465</v>
+      </c>
+      <c r="V2" s="37">
+        <v>43830</v>
+      </c>
+      <c r="W2" s="37">
+        <v>44196</v>
+      </c>
       <c r="X2" s="37">
         <v>44561</v>
       </c>
@@ -2478,7 +2506,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="2:35" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:35" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B3" s="36" t="s">
         <v>16</v>
       </c>
@@ -2503,13 +2531,22 @@
       <c r="P3" s="38">
         <v>200.05099999999999</v>
       </c>
-      <c r="Q3" s="77">
+      <c r="Q3" s="62">
         <v>210.398</v>
       </c>
       <c r="R3" s="47">
         <f>Q3*1.08</f>
         <v>227.22984000000002</v>
       </c>
+      <c r="U3" s="38">
+        <v>327.63499999999999</v>
+      </c>
+      <c r="V3" s="38">
+        <v>399.47399999999999</v>
+      </c>
+      <c r="W3" s="38">
+        <v>500.25</v>
+      </c>
       <c r="X3" s="38">
         <f>SUM(K3:N3)</f>
         <v>608.52499999999998</v>
@@ -2519,7 +2556,7 @@
         <v>813.88283999999999</v>
       </c>
     </row>
-    <row r="4" spans="2:35" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:35" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="36" t="s">
         <v>66</v>
       </c>
@@ -2544,13 +2581,22 @@
       <c r="P4" s="38">
         <v>85.561999999999998</v>
       </c>
-      <c r="Q4" s="77">
+      <c r="Q4" s="62">
         <v>101.35599999999999</v>
       </c>
       <c r="R4" s="47">
         <f>Q4*1.13</f>
         <v>114.53227999999999</v>
       </c>
+      <c r="U4" s="38">
+        <v>92.433000000000007</v>
+      </c>
+      <c r="V4" s="38">
+        <v>131.386</v>
+      </c>
+      <c r="W4" s="38">
+        <v>180.75299999999999</v>
+      </c>
       <c r="X4" s="38">
         <f>SUM(K4:N4)</f>
         <v>254.85599999999999</v>
@@ -2560,7 +2606,7 @@
         <v>381.67228</v>
       </c>
     </row>
-    <row r="5" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>96</v>
       </c>
@@ -2596,15 +2642,27 @@
         <f t="shared" si="0"/>
         <v>311.75400000000002</v>
       </c>
-      <c r="R5" s="88">
+      <c r="R5" s="73">
         <f t="shared" si="0"/>
         <v>341.76211999999998</v>
+      </c>
+      <c r="U5" s="39">
+        <f t="shared" ref="U5:W5" si="1">U3+U4</f>
+        <v>420.06799999999998</v>
+      </c>
+      <c r="V5" s="39">
+        <f t="shared" si="1"/>
+        <v>530.86</v>
+      </c>
+      <c r="W5" s="39">
+        <f t="shared" si="1"/>
+        <v>681.00299999999993</v>
       </c>
       <c r="X5" s="39">
         <f>X3+X4</f>
         <v>863.38099999999997</v>
       </c>
-      <c r="Y5" s="88">
+      <c r="Y5" s="73">
         <f>Y3+Y4</f>
         <v>1195.55512</v>
       </c>
@@ -2613,43 +2671,43 @@
         <v>1673.7771679999998</v>
       </c>
       <c r="AA5" s="39">
-        <f t="shared" ref="AA5:AI5" si="1">Z5*(1+AA21)</f>
+        <f t="shared" ref="AA5:AI5" si="2">Z5*(1+AA21)</f>
         <v>2343.2880351999997</v>
       </c>
       <c r="AB5" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3233.7374885759996</v>
       </c>
       <c r="AC5" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4397.8829844633592</v>
       </c>
       <c r="AD5" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5981.1208588701684</v>
       </c>
       <c r="AE5" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8074.5131594747281</v>
       </c>
       <c r="AF5" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10900.592765290883</v>
       </c>
       <c r="AG5" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14715.800233142692</v>
       </c>
       <c r="AH5" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19866.330314742638</v>
       </c>
       <c r="AI5" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26819.545924902563</v>
       </c>
     </row>
-    <row r="6" spans="2:35" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:35" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="36" t="s">
         <v>67</v>
       </c>
@@ -2674,18 +2732,26 @@
       <c r="P6" s="38">
         <v>87.501999999999995</v>
       </c>
-      <c r="Q6" s="77">
+      <c r="Q6" s="62">
         <v>93.724000000000004</v>
       </c>
       <c r="R6" s="48"/>
-      <c r="U6" s="90"/>
+      <c r="U6" s="38">
+        <v>139.33699999999999</v>
+      </c>
+      <c r="V6" s="38">
+        <v>190.68299999999999</v>
+      </c>
+      <c r="W6" s="38">
+        <v>224.131</v>
+      </c>
       <c r="X6" s="38">
         <f>SUM(K6:N6)</f>
         <v>260.09799999999996</v>
       </c>
       <c r="Y6" s="47"/>
     </row>
-    <row r="7" spans="2:35" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:35" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B7" s="36" t="s">
         <v>68</v>
       </c>
@@ -2710,17 +2776,26 @@
       <c r="P7" s="38">
         <v>24.148</v>
       </c>
-      <c r="Q7" s="77">
+      <c r="Q7" s="62">
         <v>24.773</v>
       </c>
       <c r="R7" s="48"/>
+      <c r="U7" s="38">
+        <v>22.148</v>
+      </c>
+      <c r="V7" s="38">
+        <v>32.890999999999998</v>
+      </c>
+      <c r="W7" s="38">
+        <v>40.540999999999997</v>
+      </c>
       <c r="X7" s="38">
         <f>SUM(K7:N7)</f>
         <v>62.373000000000005</v>
       </c>
       <c r="Y7" s="47"/>
     </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>95</v>
       </c>
@@ -2729,7 +2804,7 @@
         <v>84.834000000000003</v>
       </c>
       <c r="K8" s="40">
-        <f t="shared" ref="K8" si="2">K6+K7</f>
+        <f t="shared" ref="K8" si="3">K6+K7</f>
         <v>71.665999999999997</v>
       </c>
       <c r="L8" s="40">
@@ -2737,7 +2812,7 @@
         <v>80.866</v>
       </c>
       <c r="M8" s="40">
-        <f t="shared" ref="M8" si="3">M6+M7</f>
+        <f t="shared" ref="M8" si="4">M6+M7</f>
         <v>87.421999999999997</v>
       </c>
       <c r="N8" s="40">
@@ -2753,13 +2828,25 @@
         <v>111.64999999999999</v>
       </c>
       <c r="Q8" s="40">
-        <f t="shared" ref="Q8" si="4">Q6+Q7</f>
+        <f t="shared" ref="Q8" si="5">Q6+Q7</f>
         <v>118.497</v>
       </c>
       <c r="R8" s="47">
         <f>R5*(1-R28)</f>
         <v>129.8696056</v>
       </c>
+      <c r="U8" s="40">
+        <f t="shared" ref="U8" si="6">U6+U7</f>
+        <v>161.48499999999999</v>
+      </c>
+      <c r="V8" s="40">
+        <f t="shared" ref="V8:W8" si="7">V6+V7</f>
+        <v>223.57399999999998</v>
+      </c>
+      <c r="W8" s="40">
+        <f t="shared" si="7"/>
+        <v>264.67200000000003</v>
+      </c>
       <c r="X8" s="40">
         <f>X6+X7</f>
         <v>322.47099999999995</v>
@@ -2773,43 +2860,43 @@
         <v>636.03532383999993</v>
       </c>
       <c r="AA8" s="40">
-        <f t="shared" ref="AA8:AI8" si="5">AA5*(1-AA28)</f>
+        <f t="shared" ref="AA8:AI8" si="8">AA5*(1-AA28)</f>
         <v>867.01657302399985</v>
       </c>
       <c r="AB8" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1196.4828707731199</v>
       </c>
       <c r="AC8" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1627.2167042514429</v>
       </c>
       <c r="AD8" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2213.0147177819622</v>
       </c>
       <c r="AE8" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2987.5698690056493</v>
       </c>
       <c r="AF8" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4033.2193231576266</v>
       </c>
       <c r="AG8" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5444.8460862627962</v>
       </c>
       <c r="AH8" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>7350.5422164547763</v>
       </c>
       <c r="AI8" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>9923.2319922139486</v>
       </c>
     </row>
-    <row r="9" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>69</v>
       </c>
@@ -2818,7 +2905,7 @@
         <v>141.30600000000001</v>
       </c>
       <c r="K9" s="39">
-        <f t="shared" ref="K9" si="6">K5-K8</f>
+        <f t="shared" ref="K9" si="9">K5-K8</f>
         <v>123.35300000000001</v>
       </c>
       <c r="L9" s="39">
@@ -2826,7 +2913,7 @@
         <v>137.92899999999997</v>
       </c>
       <c r="M9" s="39">
-        <f t="shared" ref="M9" si="7">M5-M8</f>
+        <f t="shared" ref="M9" si="10">M5-M8</f>
         <v>144.56700000000001</v>
       </c>
       <c r="N9" s="39">
@@ -2842,18 +2929,30 @@
         <v>173.96300000000002</v>
       </c>
       <c r="Q9" s="39">
-        <f t="shared" ref="Q9:R9" si="8">Q5-Q8</f>
+        <f t="shared" ref="Q9:R9" si="11">Q5-Q8</f>
         <v>193.25700000000001</v>
       </c>
-      <c r="R9" s="88">
-        <f t="shared" si="8"/>
+      <c r="R9" s="73">
+        <f t="shared" si="11"/>
         <v>211.89251439999998</v>
+      </c>
+      <c r="U9" s="39">
+        <f t="shared" ref="U9" si="12">U5-U8</f>
+        <v>258.58299999999997</v>
+      </c>
+      <c r="V9" s="39">
+        <f t="shared" ref="V9:W9" si="13">V5-V8</f>
+        <v>307.28600000000006</v>
+      </c>
+      <c r="W9" s="39">
+        <f t="shared" si="13"/>
+        <v>416.3309999999999</v>
       </c>
       <c r="X9" s="39">
         <f>X5-X8</f>
         <v>540.91000000000008</v>
       </c>
-      <c r="Y9" s="88">
+      <c r="Y9" s="73">
         <f>Y5-Y8</f>
         <v>734.85151440000004</v>
       </c>
@@ -2862,43 +2961,43 @@
         <v>1037.7418441599998</v>
       </c>
       <c r="AA9" s="39">
-        <f t="shared" ref="AA9:AI9" si="9">AA5-AA8</f>
+        <f t="shared" ref="AA9:AI9" si="14">AA5-AA8</f>
         <v>1476.2714621759999</v>
       </c>
       <c r="AB9" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>2037.2546178028797</v>
       </c>
       <c r="AC9" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>2770.6662802119163</v>
       </c>
       <c r="AD9" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3768.1061410882062</v>
       </c>
       <c r="AE9" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>5086.9432904690784</v>
       </c>
       <c r="AF9" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>6867.3734421332565</v>
       </c>
       <c r="AG9" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>9270.9541468798961</v>
       </c>
       <c r="AH9" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>12515.788098287861</v>
       </c>
       <c r="AI9" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>16896.313932688616</v>
       </c>
     </row>
-    <row r="10" spans="2:35" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:35" s="40" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B10" s="40" t="s">
         <v>70</v>
       </c>
@@ -2923,15 +3022,22 @@
       <c r="P10" s="40">
         <v>95.004999999999995</v>
       </c>
-      <c r="Q10" s="79">
+      <c r="Q10" s="64">
         <v>102.023</v>
       </c>
       <c r="R10" s="47">
         <f>R9*0.58</f>
         <v>122.89765835199998</v>
       </c>
-      <c r="V10" s="96"/>
-      <c r="W10" s="96"/>
+      <c r="U10" s="40">
+        <v>156.886</v>
+      </c>
+      <c r="V10" s="40">
+        <v>212.959</v>
+      </c>
+      <c r="W10" s="40">
+        <v>307.286</v>
+      </c>
       <c r="X10" s="40">
         <f>SUM(K10:N10)</f>
         <v>515.00700000000006</v>
@@ -2941,47 +3047,47 @@
         <v>410.05465835200005</v>
       </c>
       <c r="Z10" s="40">
-        <f>Z9*0.55</f>
-        <v>570.75801428799991</v>
+        <f t="shared" ref="Z10:AI10" si="15">Z9*0.65</f>
+        <v>674.53219870399994</v>
       </c>
       <c r="AA10" s="40">
-        <f t="shared" ref="AA10:AI10" si="10">AA9*0.65</f>
+        <f t="shared" si="15"/>
         <v>959.57645041439991</v>
       </c>
       <c r="AB10" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1324.2155015718718</v>
       </c>
       <c r="AC10" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>1800.9330821377457</v>
       </c>
       <c r="AD10" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>2449.268991707334</v>
       </c>
       <c r="AE10" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>3306.5131388049012</v>
       </c>
       <c r="AF10" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>4463.7927373866169</v>
       </c>
       <c r="AG10" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>6026.1201954719327</v>
       </c>
       <c r="AH10" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8135.2622638871098</v>
       </c>
       <c r="AI10" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>10982.604056247601</v>
       </c>
     </row>
-    <row r="11" spans="2:35" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:35" s="40" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B11" s="40" t="s">
         <v>71</v>
       </c>
@@ -3006,101 +3112,122 @@
       <c r="P11" s="40">
         <v>57.546999999999997</v>
       </c>
-      <c r="Q11" s="79">
+      <c r="Q11" s="64">
         <v>59.127000000000002</v>
       </c>
       <c r="R11" s="47">
         <f>R9*R33</f>
-        <v>42.378502879999999</v>
+        <v>44.497428023999994</v>
+      </c>
+      <c r="U11" s="40">
+        <v>76.855999999999995</v>
+      </c>
+      <c r="V11" s="40">
+        <v>100.721</v>
+      </c>
+      <c r="W11" s="40">
+        <v>123.19499999999999</v>
       </c>
       <c r="X11" s="40">
-        <f t="shared" ref="X11:X16" si="11">SUM(K11:N11)</f>
+        <f t="shared" ref="X11:X16" si="16">SUM(K11:N11)</f>
         <v>194.02600000000001</v>
       </c>
       <c r="Y11" s="47">
         <f>SUM(O11:R11)</f>
-        <v>207.46850288000002</v>
+        <v>209.58742802399999</v>
       </c>
       <c r="Z11" s="40">
         <f>Z5*Z33</f>
         <v>318.01766191999997</v>
       </c>
       <c r="AA11" s="40">
-        <f t="shared" ref="AA11:AI11" si="12">AA5*AA33</f>
+        <f t="shared" ref="AA11:AI11" si="17">AA5*AA33</f>
         <v>468.65760703999996</v>
       </c>
       <c r="AB11" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>646.74749771519998</v>
       </c>
       <c r="AC11" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>879.57659689267189</v>
       </c>
       <c r="AD11" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>1196.2241717740337</v>
       </c>
       <c r="AE11" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>1614.9026318949457</v>
       </c>
       <c r="AF11" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>1962.106697752359</v>
       </c>
       <c r="AG11" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>2648.8440419656845</v>
       </c>
       <c r="AH11" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>3575.9394566536748</v>
       </c>
       <c r="AI11" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>4827.5182664824615</v>
       </c>
     </row>
-    <row r="12" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
         <v>72</v>
       </c>
       <c r="J12" s="40">
-        <f t="shared" ref="J12:P12" si="13">J10+J11</f>
+        <f t="shared" ref="J12:P12" si="18">J10+J11</f>
         <v>135.53100000000001</v>
       </c>
       <c r="K12" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>173.61500000000001</v>
       </c>
       <c r="L12" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>231.614</v>
       </c>
       <c r="M12" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>141.67699999999999</v>
       </c>
       <c r="N12" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>162.12700000000001</v>
       </c>
       <c r="O12" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>138.54500000000002</v>
       </c>
       <c r="P12" s="40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>152.55199999999999</v>
       </c>
       <c r="Q12" s="40">
-        <f t="shared" ref="Q12:R12" si="14">Q10+Q11</f>
+        <f t="shared" ref="Q12:R12" si="19">Q10+Q11</f>
         <v>161.15</v>
       </c>
       <c r="R12" s="47">
-        <f t="shared" si="14"/>
-        <v>165.27616123199999</v>
+        <f t="shared" si="19"/>
+        <v>167.39508637599997</v>
+      </c>
+      <c r="U12" s="40">
+        <f t="shared" ref="U12:V12" si="20">U10+U11</f>
+        <v>233.74199999999999</v>
+      </c>
+      <c r="V12" s="40">
+        <f t="shared" si="20"/>
+        <v>313.68</v>
+      </c>
+      <c r="W12" s="40">
+        <f t="shared" ref="W12" si="21">W10+W11</f>
+        <v>430.48099999999999</v>
       </c>
       <c r="X12" s="40">
         <f>X10+X11</f>
@@ -3108,50 +3235,50 @@
       </c>
       <c r="Y12" s="47">
         <f>Y10+Y11</f>
-        <v>617.52316123200012</v>
+        <v>619.64208637600007</v>
       </c>
       <c r="Z12" s="40">
-        <f t="shared" ref="Z12:AI12" si="15">Z10+Z11</f>
-        <v>888.77567620799982</v>
+        <f t="shared" ref="Z12:AI12" si="22">Z10+Z11</f>
+        <v>992.54986062399985</v>
       </c>
       <c r="AA12" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>1428.2340574543998</v>
       </c>
       <c r="AB12" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>1970.9629992870719</v>
       </c>
       <c r="AC12" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>2680.5096790304178</v>
       </c>
       <c r="AD12" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>3645.4931634813674</v>
       </c>
       <c r="AE12" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>4921.4157706998467</v>
       </c>
       <c r="AF12" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>6425.8994351389756</v>
       </c>
       <c r="AG12" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>8674.9642374376162</v>
       </c>
       <c r="AH12" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>11711.201720540785</v>
       </c>
       <c r="AI12" s="40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>15810.122322730062</v>
       </c>
     </row>
-    <row r="13" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B13" s="2" t="s">
         <v>73</v>
       </c>
@@ -3159,87 +3286,99 @@
         <v>5.7750000000000004</v>
       </c>
       <c r="K13" s="39">
-        <f t="shared" ref="K13:P13" si="16">K9-K12</f>
+        <f t="shared" ref="K13:P13" si="23">K9-K12</f>
         <v>-50.262</v>
       </c>
       <c r="L13" s="39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>-93.685000000000031</v>
       </c>
       <c r="M13" s="39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>2.8900000000000148</v>
       </c>
       <c r="N13" s="39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>-27.066000000000031</v>
       </c>
       <c r="O13" s="39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>17.19399999999996</v>
       </c>
       <c r="P13" s="39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>21.41100000000003</v>
       </c>
       <c r="Q13" s="39">
-        <f t="shared" ref="Q13:R13" si="17">Q9-Q12</f>
+        <f t="shared" ref="Q13:R13" si="24">Q9-Q12</f>
         <v>32.106999999999999</v>
       </c>
-      <c r="R13" s="88">
-        <f t="shared" si="17"/>
-        <v>46.616353167999989</v>
+      <c r="R13" s="73">
+        <f t="shared" si="24"/>
+        <v>44.497428024000016</v>
+      </c>
+      <c r="U13" s="39">
+        <f t="shared" ref="U13:V13" si="25">U9-U12</f>
+        <v>24.84099999999998</v>
+      </c>
+      <c r="V13" s="39">
+        <f t="shared" si="25"/>
+        <v>-6.3939999999999486</v>
+      </c>
+      <c r="W13" s="39">
+        <f t="shared" ref="W13" si="26">W9-W12</f>
+        <v>-14.150000000000091</v>
       </c>
       <c r="X13" s="39">
         <f>X9-X12</f>
         <v>-168.12300000000005</v>
       </c>
-      <c r="Y13" s="88">
+      <c r="Y13" s="73">
         <f>Y9-Y12</f>
-        <v>117.32835316799992</v>
+        <v>115.20942802399998</v>
       </c>
       <c r="Z13" s="39">
         <f>Z9-Z12</f>
-        <v>148.96616795199998</v>
+        <v>45.191983535999952</v>
       </c>
       <c r="AA13" s="39">
-        <f t="shared" ref="AA13:AI13" si="18">AA9-AA12</f>
+        <f t="shared" ref="AA13:AI13" si="27">AA9-AA12</f>
         <v>48.037404721600069</v>
       </c>
       <c r="AB13" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>66.291618515807841</v>
       </c>
       <c r="AC13" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>90.156601181498445</v>
       </c>
       <c r="AD13" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>122.61297760683874</v>
       </c>
       <c r="AE13" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>165.52751976923173</v>
       </c>
       <c r="AF13" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>441.4740069942809</v>
       </c>
       <c r="AG13" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>595.9899094422799</v>
       </c>
       <c r="AH13" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>804.58637774707677</v>
       </c>
       <c r="AI13" s="39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>1086.1916099585542</v>
       </c>
     </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>74</v>
       </c>
@@ -3264,15 +3403,24 @@
       <c r="P14" s="40">
         <v>47.026000000000003</v>
       </c>
-      <c r="Q14" s="79">
+      <c r="Q14" s="64">
         <v>-11.249000000000001</v>
       </c>
       <c r="R14" s="47">
         <f>AVERAGE(N14:Q14)</f>
         <v>20.231999999999999</v>
       </c>
+      <c r="U14" s="40">
+        <v>3.2629999999999999</v>
+      </c>
+      <c r="V14" s="40">
+        <v>8.4640000000000004</v>
+      </c>
+      <c r="W14" s="40">
+        <v>7.859</v>
+      </c>
       <c r="X14" s="40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>26.748000000000001</v>
       </c>
       <c r="Y14" s="47">
@@ -3284,81 +3432,93 @@
         <v>69.028000000000006</v>
       </c>
       <c r="AA14" s="40">
-        <f t="shared" ref="AA14:AI14" si="19">AVERAGE(Y14:Z14)</f>
+        <f t="shared" ref="AA14:AI14" si="28">AVERAGE(Y14:Z14)</f>
         <v>90.168000000000006</v>
       </c>
       <c r="AB14" s="40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>79.598000000000013</v>
       </c>
       <c r="AC14" s="40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>84.88300000000001</v>
       </c>
       <c r="AD14" s="40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>82.240500000000011</v>
       </c>
       <c r="AE14" s="40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>83.561750000000018</v>
       </c>
       <c r="AF14" s="40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>82.901125000000008</v>
       </c>
       <c r="AG14" s="40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>83.231437500000013</v>
       </c>
       <c r="AH14" s="40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>83.066281250000003</v>
       </c>
       <c r="AI14" s="40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>83.148859375000001</v>
       </c>
     </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>75</v>
       </c>
       <c r="J15" s="40">
-        <f t="shared" ref="J15:Q15" si="20">J13+J14</f>
+        <f t="shared" ref="J15:Q15" si="29">J13+J14</f>
         <v>9.0400000000000009</v>
       </c>
       <c r="K15" s="40">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-49.677</v>
       </c>
       <c r="L15" s="40">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-51.84400000000003</v>
       </c>
       <c r="M15" s="40">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-2.6399999999999855</v>
       </c>
       <c r="N15" s="40">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>-37.214000000000027</v>
       </c>
       <c r="O15" s="40">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>72.492999999999967</v>
       </c>
       <c r="P15" s="40">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>68.43700000000004</v>
       </c>
       <c r="Q15" s="40">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>20.857999999999997</v>
       </c>
       <c r="R15" s="47">
         <f>R13+R14</f>
-        <v>66.848353167999989</v>
+        <v>64.729428024000015</v>
+      </c>
+      <c r="U15" s="40">
+        <f t="shared" ref="U15:W15" si="30">U13+U14</f>
+        <v>28.103999999999978</v>
+      </c>
+      <c r="V15" s="40">
+        <f t="shared" si="30"/>
+        <v>2.0700000000000518</v>
+      </c>
+      <c r="W15" s="40">
+        <f t="shared" si="30"/>
+        <v>-6.291000000000091</v>
       </c>
       <c r="X15" s="40">
         <f>X13+X14</f>
@@ -3366,50 +3526,50 @@
       </c>
       <c r="Y15" s="47">
         <f>Y13+Y14</f>
-        <v>228.63635316799991</v>
+        <v>226.51742802399997</v>
       </c>
       <c r="Z15" s="40">
         <f>Z13+Z14</f>
-        <v>217.994167952</v>
+        <v>114.21998353599996</v>
       </c>
       <c r="AA15" s="40">
-        <f t="shared" ref="AA15:AI15" si="21">AA13+AA14</f>
+        <f t="shared" ref="AA15:AI15" si="31">AA13+AA14</f>
         <v>138.20540472160008</v>
       </c>
       <c r="AB15" s="40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>145.88961851580785</v>
       </c>
       <c r="AC15" s="40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>175.03960118149845</v>
       </c>
       <c r="AD15" s="40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>204.85347760683874</v>
       </c>
       <c r="AE15" s="40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>249.08926976923175</v>
       </c>
       <c r="AF15" s="40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>524.37513199428088</v>
       </c>
       <c r="AG15" s="40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>679.22134694227987</v>
       </c>
       <c r="AH15" s="40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>887.65265899707674</v>
       </c>
       <c r="AI15" s="40">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>1169.3404693335542</v>
       </c>
     </row>
-    <row r="16" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>76</v>
       </c>
@@ -3434,148 +3594,169 @@
       <c r="P16" s="40">
         <v>17.475000000000001</v>
       </c>
-      <c r="Q16" s="79">
+      <c r="Q16" s="64">
         <v>8.7270000000000003</v>
       </c>
       <c r="R16" s="47">
         <f>R13*R31</f>
-        <v>19.112704798879996</v>
+        <v>18.243945489840005</v>
+      </c>
+      <c r="U16" s="40">
+        <v>-1.101</v>
+      </c>
+      <c r="V16" s="40">
+        <v>1.1879999999999999</v>
+      </c>
+      <c r="W16" s="40">
+        <v>-4.5670000000000002</v>
       </c>
       <c r="X16" s="40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>-81.356999999999999</v>
       </c>
       <c r="Y16" s="47">
         <f>SUM(O16:R16)</f>
-        <v>62.97670479888</v>
+        <v>62.107945489840006</v>
       </c>
       <c r="Z16" s="40">
         <f>Z15*Z31</f>
-        <v>87.197667180800011</v>
+        <v>46.830193249759979</v>
       </c>
       <c r="AA16" s="40">
-        <f t="shared" ref="AA16:AI16" si="22">AA15*AA31</f>
-        <v>59.428324030288032</v>
+        <f t="shared" ref="AA16:AI16" si="32">AA15*AA31</f>
+        <v>58.04626998307203</v>
       </c>
       <c r="AB16" s="40">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>62.732535961797375</v>
       </c>
       <c r="AC16" s="40">
-        <f t="shared" si="22"/>
-        <v>78.767820531674303</v>
+        <f t="shared" si="32"/>
+        <v>84.019008567119258</v>
       </c>
       <c r="AD16" s="40">
-        <f t="shared" si="22"/>
-        <v>92.184064923077429</v>
+        <f t="shared" si="32"/>
+        <v>98.329669251282596</v>
       </c>
       <c r="AE16" s="40">
-        <f t="shared" si="22"/>
-        <v>112.09017139615429</v>
+        <f t="shared" si="32"/>
+        <v>139.4899910707698</v>
       </c>
       <c r="AF16" s="40">
-        <f t="shared" si="22"/>
-        <v>235.96880939742641</v>
+        <f t="shared" si="32"/>
+        <v>298.8938252367401</v>
       </c>
       <c r="AG16" s="40">
-        <f t="shared" si="22"/>
-        <v>305.64960612402592</v>
+        <f t="shared" si="32"/>
+        <v>393.94838122652232</v>
       </c>
       <c r="AH16" s="40">
-        <f t="shared" si="22"/>
-        <v>399.44369654868456</v>
+        <f t="shared" si="32"/>
+        <v>523.7150688082753</v>
       </c>
       <c r="AI16" s="40">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>526.20321120009942</v>
       </c>
     </row>
-    <row r="17" spans="2:73" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:73" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J17" s="39">
-        <f t="shared" ref="J17:Q17" si="23">J15-J16</f>
+        <f t="shared" ref="J17:Q17" si="33">J15-J16</f>
         <v>25.834000000000003</v>
       </c>
       <c r="K17" s="39">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>-47.917000000000002</v>
       </c>
       <c r="L17" s="39">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>-47.117000000000033</v>
       </c>
       <c r="M17" s="39">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>48.524000000000015</v>
       </c>
       <c r="N17" s="39">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>-13.508000000000028</v>
       </c>
       <c r="O17" s="39">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>54.830999999999968</v>
       </c>
       <c r="P17" s="39">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>50.962000000000039</v>
       </c>
       <c r="Q17" s="39">
-        <f t="shared" si="23"/>
+        <f t="shared" si="33"/>
         <v>12.130999999999997</v>
       </c>
-      <c r="R17" s="88">
+      <c r="R17" s="73">
         <f>R15-R16</f>
-        <v>47.735648369119993</v>
+        <v>46.485482534160013</v>
+      </c>
+      <c r="U17" s="39">
+        <f t="shared" ref="U17:W17" si="34">U15-U16</f>
+        <v>29.204999999999977</v>
+      </c>
+      <c r="V17" s="39">
+        <f t="shared" si="34"/>
+        <v>0.88200000000005185</v>
+      </c>
+      <c r="W17" s="39">
+        <f t="shared" si="34"/>
+        <v>-1.7240000000000908</v>
       </c>
       <c r="X17" s="39">
         <f>X15-X16</f>
         <v>-60.018000000000058</v>
       </c>
-      <c r="Y17" s="88">
+      <c r="Y17" s="73">
         <f>Y15-Y16</f>
-        <v>165.65964836911991</v>
+        <v>164.40948253415996</v>
       </c>
       <c r="Z17" s="39">
         <f>Z15-Z16</f>
-        <v>130.79650077119999</v>
+        <v>67.389790286239986</v>
       </c>
       <c r="AA17" s="39">
-        <f t="shared" ref="AA17:AI17" si="24">AA15-AA16</f>
-        <v>78.777080691312051</v>
+        <f t="shared" ref="AA17:AI17" si="35">AA15-AA16</f>
+        <v>80.159134738528053</v>
       </c>
       <c r="AB17" s="39">
-        <f t="shared" si="24"/>
+        <f t="shared" si="35"/>
         <v>83.157082554010486</v>
       </c>
       <c r="AC17" s="39">
-        <f t="shared" si="24"/>
-        <v>96.271780649824152</v>
+        <f t="shared" si="35"/>
+        <v>91.020592614379197</v>
       </c>
       <c r="AD17" s="39">
-        <f t="shared" si="24"/>
-        <v>112.66941268376131</v>
+        <f t="shared" si="35"/>
+        <v>106.52380835555614</v>
       </c>
       <c r="AE17" s="39">
-        <f t="shared" si="24"/>
-        <v>136.99909837307746</v>
+        <f t="shared" si="35"/>
+        <v>109.59927869846194</v>
       </c>
       <c r="AF17" s="39">
-        <f t="shared" si="24"/>
-        <v>288.40632259685447</v>
+        <f t="shared" si="35"/>
+        <v>225.48130675754078</v>
       </c>
       <c r="AG17" s="39">
-        <f t="shared" si="24"/>
-        <v>373.57174081825394</v>
+        <f t="shared" si="35"/>
+        <v>285.27296571575755</v>
       </c>
       <c r="AH17" s="39">
-        <f t="shared" si="24"/>
-        <v>488.20896244839219</v>
+        <f t="shared" si="35"/>
+        <v>363.93759018880144</v>
       </c>
       <c r="AI17" s="39">
-        <f t="shared" si="24"/>
+        <f t="shared" si="35"/>
         <v>643.13725813345479</v>
       </c>
       <c r="AJ17" s="39">
@@ -3583,204 +3764,216 @@
         <v>675.29412104012761</v>
       </c>
       <c r="AK17" s="39">
-        <f t="shared" ref="AK17:BU17" si="25">AJ17*(1+$AL$21)</f>
+        <f t="shared" ref="AK17:BU17" si="36">AJ17*(1+$AL$21)</f>
         <v>709.05882709213404</v>
       </c>
       <c r="AL17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>744.5117684467408</v>
       </c>
       <c r="AM17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>781.73735686907787</v>
       </c>
       <c r="AN17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>820.82422471253176</v>
       </c>
       <c r="AO17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>861.86543594815839</v>
       </c>
       <c r="AP17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>904.95870774556636</v>
       </c>
       <c r="AQ17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>950.20664313284476</v>
       </c>
       <c r="AR17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>997.7169752894871</v>
       </c>
       <c r="AS17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1047.6028240539615</v>
       </c>
       <c r="AT17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1099.9829652566596</v>
       </c>
       <c r="AU17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1154.9821135194925</v>
       </c>
       <c r="AV17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1212.7312191954672</v>
       </c>
       <c r="AW17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1273.3677801552406</v>
       </c>
       <c r="AX17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1337.0361691630026</v>
       </c>
       <c r="AY17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1403.8879776211527</v>
       </c>
       <c r="AZ17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1474.0823765022103</v>
       </c>
       <c r="BA17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1547.7864953273208</v>
       </c>
       <c r="BB17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1625.175820093687</v>
       </c>
       <c r="BC17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1706.4346110983713</v>
       </c>
       <c r="BD17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1791.7563416532898</v>
       </c>
       <c r="BE17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1881.3441587359544</v>
       </c>
       <c r="BF17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>1975.4113666727521</v>
       </c>
       <c r="BG17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>2074.1819350063897</v>
       </c>
       <c r="BH17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>2177.8910317567093</v>
       </c>
       <c r="BI17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>2286.7855833445446</v>
       </c>
       <c r="BJ17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>2401.1248625117719</v>
       </c>
       <c r="BK17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>2521.1811056373604</v>
       </c>
       <c r="BL17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>2647.2401609192284</v>
       </c>
       <c r="BM17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>2779.6021689651898</v>
       </c>
       <c r="BN17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>2918.5822774134494</v>
       </c>
       <c r="BO17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>3064.5113912841221</v>
       </c>
       <c r="BP17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>3217.7369608483282</v>
       </c>
       <c r="BQ17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>3378.6238088907448</v>
       </c>
       <c r="BR17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>3547.5549993352824</v>
       </c>
       <c r="BS17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>3724.9327493020469</v>
       </c>
       <c r="BT17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>3911.1793867671495</v>
       </c>
       <c r="BU17" s="39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="36"/>
         <v>4106.7383561055067</v>
       </c>
     </row>
-    <row r="18" spans="2:73" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:73" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J18" s="43">
-        <f t="shared" ref="J18:Q18" si="26">J17/J19</f>
+        <f t="shared" ref="J18:Q18" si="37">J17/J19</f>
         <v>0.40594603937836865</v>
       </c>
       <c r="K18" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>-0.74828221625335745</v>
       </c>
       <c r="L18" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>-0.72303041463339834</v>
       </c>
       <c r="M18" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>0.73307952622673467</v>
       </c>
       <c r="N18" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>-0.19489251190304469</v>
       </c>
       <c r="O18" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>0.77281183932346675</v>
       </c>
       <c r="P18" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>0.71737049549549603</v>
       </c>
       <c r="Q18" s="43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="37"/>
         <v>0.17060205043104049</v>
       </c>
-      <c r="R18" s="86">
+      <c r="R18" s="71">
         <f>R17/R19</f>
-        <v>0.67132136595721925</v>
+        <v>0.65373989247415887</v>
+      </c>
+      <c r="U18" s="43">
+        <f t="shared" ref="U18:W18" si="38">U17/U19</f>
+        <v>0.51789260888069188</v>
+      </c>
+      <c r="V18" s="43">
+        <f t="shared" si="38"/>
+        <v>1.4901165737456527E-2</v>
+      </c>
+      <c r="W18" s="43">
+        <f t="shared" si="38"/>
+        <v>-2.6657145550691104E-2</v>
       </c>
       <c r="X18" s="43">
         <f>X17/X19</f>
         <v>-0.86593565142115214</v>
       </c>
-      <c r="Y18" s="91">
+      <c r="Y18" s="75">
         <f>Y17/Y19</f>
-        <v>2.3297234923301491</v>
-      </c>
-    </row>
-    <row r="19" spans="2:73" x14ac:dyDescent="0.2">
+        <v>2.3121420188470889</v>
+      </c>
+    </row>
+    <row r="19" spans="2:73" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
@@ -3812,13 +4005,22 @@
       <c r="P19" s="40">
         <v>71.040000000000006</v>
       </c>
-      <c r="Q19" s="79">
+      <c r="Q19" s="64">
         <v>71.106999999999999</v>
       </c>
       <c r="R19" s="47">
         <f>Q19</f>
         <v>71.106999999999999</v>
       </c>
+      <c r="U19" s="40">
+        <v>56.392000000000003</v>
+      </c>
+      <c r="V19" s="40">
+        <v>59.19</v>
+      </c>
+      <c r="W19" s="40">
+        <v>64.673090999999999</v>
+      </c>
       <c r="X19" s="40">
         <f>N19</f>
         <v>69.31</v>
@@ -3828,7 +4030,7 @@
         <v>71.106999999999999</v>
       </c>
     </row>
-    <row r="21" spans="2:73" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:73" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>79</v>
       </c>
@@ -3838,7 +4040,7 @@
         <v>-3.786150172459557E-2</v>
       </c>
       <c r="O21" s="42">
-        <f t="shared" ref="O21" si="27">O5/K5-1</f>
+        <f t="shared" ref="O21" si="39">O5/K5-1</f>
         <v>0.31487701198344764</v>
       </c>
       <c r="P21" s="42">
@@ -3846,11 +4048,26 @@
         <v>0.30539089101670513</v>
       </c>
       <c r="Q21" s="42">
-        <f t="shared" ref="Q21" si="28">Q5/M5-1</f>
+        <f t="shared" ref="Q21" si="40">Q5/M5-1</f>
         <v>0.34383095750229553</v>
       </c>
-      <c r="R21" s="85"/>
-      <c r="Y21" s="89">
+      <c r="R21" s="70"/>
+      <c r="U21" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="V21" s="42">
+        <f t="shared" ref="V21:W21" si="41">V5/U5-1</f>
+        <v>0.26374777416989637</v>
+      </c>
+      <c r="W21" s="42">
+        <f t="shared" ref="V21:X21" si="42">W5/V5-1</f>
+        <v>0.28282974795614657</v>
+      </c>
+      <c r="X21" s="42">
+        <f>X5/W5-1</f>
+        <v>0.26780792448785107</v>
+      </c>
+      <c r="Y21" s="74">
         <f>Y5/X5-1</f>
         <v>0.38473642574946632</v>
       </c>
@@ -3884,14 +4101,14 @@
       <c r="AI21" s="42">
         <v>0.35</v>
       </c>
-      <c r="AK21" s="93" t="s">
-        <v>169</v>
-      </c>
-      <c r="AL21" s="41">
+      <c r="AK21" s="92" t="s">
+        <v>168</v>
+      </c>
+      <c r="AL21" s="93">
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="36" t="s">
         <v>92</v>
       </c>
@@ -3901,7 +4118,7 @@
         <v>-0.16487284339176189</v>
       </c>
       <c r="O22" s="44">
-        <f t="shared" ref="O22:O23" si="29">O3/K3-1</f>
+        <f t="shared" ref="O22:O23" si="43">O3/K3-1</f>
         <v>0.25068495095325316</v>
       </c>
       <c r="P22" s="44">
@@ -3909,71 +4126,101 @@
         <v>0.27887768735576346</v>
       </c>
       <c r="Q22" s="44">
-        <f t="shared" ref="Q22:Q23" si="30">Q3/M3-1</f>
+        <f t="shared" ref="Q22:Q23" si="44">Q3/M3-1</f>
         <v>0.26896377025747431</v>
       </c>
       <c r="R22" s="48"/>
+      <c r="U22" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="V22" s="44">
+        <f t="shared" ref="V22:W22" si="45">V3/U3-1</f>
+        <v>0.21926534100447137</v>
+      </c>
+      <c r="W22" s="44">
+        <f t="shared" ref="V22:X22" si="46">W3/V3-1</f>
+        <v>0.25227173733459507</v>
+      </c>
+      <c r="X22" s="44">
+        <f>X3/W3-1</f>
+        <v>0.21644177911044471</v>
+      </c>
       <c r="Y22" s="48"/>
-      <c r="AK22" s="93" t="s">
-        <v>170</v>
-      </c>
-      <c r="AL22" s="44">
+      <c r="AK22" s="94" t="s">
+        <v>169</v>
+      </c>
+      <c r="AL22" s="95">
         <v>0.06</v>
       </c>
     </row>
-    <row r="23" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B23" s="36" t="s">
         <v>93</v>
       </c>
       <c r="M23" s="44"/>
       <c r="N23" s="44">
-        <f t="shared" ref="N23:P23" si="31">N4/J4-1</f>
+        <f t="shared" ref="N23:P23" si="47">N4/J4-1</f>
         <v>0.38722512686452393</v>
       </c>
       <c r="O23" s="44">
-        <f t="shared" si="29"/>
+        <f t="shared" si="43"/>
         <v>0.48194262279940125</v>
       </c>
       <c r="P23" s="44">
-        <f t="shared" si="31"/>
+        <f t="shared" si="47"/>
         <v>0.3718894304771676</v>
       </c>
       <c r="Q23" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="44"/>
         <v>0.53138125887649923</v>
       </c>
       <c r="R23" s="48"/>
+      <c r="U23" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="V23" s="44">
+        <f t="shared" ref="V23:W23" si="48">V4/U4-1</f>
+        <v>0.42141875737020307</v>
+      </c>
+      <c r="W23" s="44">
+        <f t="shared" ref="V23:X23" si="49">W4/V4-1</f>
+        <v>0.37574018540788212</v>
+      </c>
+      <c r="X23" s="44">
+        <f>X4/W4-1</f>
+        <v>0.40996829928133982</v>
+      </c>
       <c r="Y23" s="48"/>
-      <c r="AK23" s="93" t="s">
-        <v>171</v>
-      </c>
-      <c r="AL23" s="39">
+      <c r="AK23" s="94" t="s">
+        <v>170</v>
+      </c>
+      <c r="AL23" s="96">
         <f>NPV(AL22,Y17:BU17)</f>
-        <v>12420.186517227328</v>
-      </c>
-    </row>
-    <row r="24" spans="2:73" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>12176.120593498938</v>
+      </c>
+    </row>
+    <row r="24" spans="2:73" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
         <v>80</v>
       </c>
       <c r="K24" s="42">
-        <f t="shared" ref="K24:L24" si="32">K5/J5-1</f>
+        <f t="shared" ref="K24:L24" si="50">K5/J5-1</f>
         <v>-0.13761828955514288</v>
       </c>
       <c r="L24" s="42">
-        <f t="shared" si="32"/>
+        <f t="shared" si="50"/>
         <v>0.12191632610155922</v>
       </c>
       <c r="M24" s="42">
-        <f t="shared" ref="M24" si="33">M5/L5-1</f>
+        <f t="shared" ref="M24" si="51">M5/L5-1</f>
         <v>6.0303023378047937E-2</v>
       </c>
       <c r="N24" s="42">
-        <f t="shared" ref="N24" si="34">N5/M5-1</f>
+        <f t="shared" ref="N24" si="52">N5/M5-1</f>
         <v>-6.2119324623150396E-2</v>
       </c>
       <c r="O24" s="42">
-        <f t="shared" ref="O24" si="35">O5/N5-1</f>
+        <f t="shared" ref="O24" si="53">O5/N5-1</f>
         <v>0.17854746343839922</v>
       </c>
       <c r="P24" s="42">
@@ -3981,46 +4228,85 @@
         <v>0.11382231131008558</v>
       </c>
       <c r="Q24" s="42">
-        <f t="shared" ref="Q24" si="36">Q5/P5-1</f>
+        <f t="shared" ref="Q24" si="54">Q5/P5-1</f>
         <v>9.1525945947838583E-2</v>
       </c>
-      <c r="R24" s="85"/>
+      <c r="R24" s="70"/>
+      <c r="U24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="V24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="W24" s="34" t="s">
+        <v>151</v>
+      </c>
       <c r="X24" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="Y24" s="92" t="s">
+      <c r="Y24" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="AK24" s="93" t="s">
+      <c r="Z24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI24" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK24" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="AL24" s="40">
+      <c r="AL24" s="97">
         <f>Main!C11</f>
         <v>377.61800000000005</v>
       </c>
     </row>
-    <row r="25" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B25" s="36" t="s">
         <v>90</v>
       </c>
       <c r="K25" s="44">
-        <f t="shared" ref="K25:L25" si="37">K3/J3-1</f>
+        <f t="shared" ref="K25:L25" si="55">K3/J3-1</f>
         <v>-0.19084977830871386</v>
       </c>
       <c r="L25" s="44">
-        <f t="shared" si="37"/>
+        <f t="shared" si="55"/>
         <v>0.1103090441917578</v>
       </c>
       <c r="M25" s="44">
-        <f t="shared" ref="M25" si="38">M3/L3-1</f>
+        <f t="shared" ref="M25" si="56">M3/L3-1</f>
         <v>5.9938501665313559E-2</v>
       </c>
       <c r="N25" s="44">
-        <f t="shared" ref="N25" si="39">N3/M3-1</f>
+        <f t="shared" ref="N25" si="57">N3/M3-1</f>
         <v>-0.1230013932196643</v>
       </c>
       <c r="O25" s="44">
-        <f t="shared" ref="O25" si="40">O3/N3-1</f>
+        <f t="shared" ref="O25" si="58">O3/N3-1</f>
         <v>0.21178193921971822</v>
       </c>
       <c r="P25" s="44">
@@ -4028,46 +4314,85 @@
         <v>0.13533744977412532</v>
       </c>
       <c r="Q25" s="44">
-        <f t="shared" ref="Q25:Q26" si="41">Q3/P3-1</f>
+        <f t="shared" ref="Q25:Q26" si="59">Q3/P3-1</f>
         <v>5.1721810938210711E-2</v>
       </c>
       <c r="R25" s="48"/>
+      <c r="U25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="V25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="W25" s="23" t="s">
+        <v>151</v>
+      </c>
       <c r="X25" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="Y25" s="92" t="s">
+      <c r="Y25" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="AK25" s="93" t="s">
-        <v>172</v>
-      </c>
-      <c r="AL25" s="40">
+      <c r="Z25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI25" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK25" s="94" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL25" s="97">
         <f>AL23-AL24</f>
-        <v>12042.568517227328</v>
-      </c>
-    </row>
-    <row r="26" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.2">
+        <v>11798.502593498937</v>
+      </c>
+    </row>
+    <row r="26" spans="2:73" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B26" s="36" t="s">
         <v>91</v>
       </c>
       <c r="K26" s="44">
-        <f t="shared" ref="K26:L26" si="42">K4/J4-1</f>
+        <f t="shared" ref="K26:L26" si="60">K4/J4-1</f>
         <v>4.053898200830397E-2</v>
       </c>
       <c r="L26" s="44">
-        <f t="shared" si="42"/>
+        <f t="shared" si="60"/>
         <v>0.15212532096872522</v>
       </c>
       <c r="M26" s="44">
-        <f t="shared" ref="M26" si="43">M4/L4-1</f>
+        <f t="shared" ref="M26" si="61">M4/L4-1</f>
         <v>6.1217290918419875E-2</v>
       </c>
       <c r="N26" s="44">
-        <f t="shared" ref="N26" si="44">N4/M4-1</f>
+        <f t="shared" ref="N26" si="62">N4/M4-1</f>
         <v>9.0396760644244845E-2</v>
       </c>
       <c r="O26" s="44">
-        <f t="shared" ref="O26" si="45">O4/N4-1</f>
+        <f t="shared" ref="O26" si="63">O4/N4-1</f>
         <v>0.1115853067106376</v>
       </c>
       <c r="P26" s="44">
@@ -4075,34 +4400,73 @@
         <v>6.6565281344269644E-2</v>
       </c>
       <c r="Q26" s="44">
-        <f t="shared" si="41"/>
+        <f t="shared" si="59"/>
         <v>0.18459129052616818</v>
       </c>
       <c r="R26" s="48"/>
+      <c r="U26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="V26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="W26" s="23" t="s">
+        <v>151</v>
+      </c>
       <c r="X26" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="Y26" s="92" t="s">
+      <c r="Y26" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="AK26" s="94" t="s">
+      <c r="Z26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI26" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK26" s="98" t="s">
+        <v>172</v>
+      </c>
+      <c r="AL26" s="99">
+        <f>AL25/Q19</f>
+        <v>165.92603531999575</v>
+      </c>
+    </row>
+    <row r="27" spans="2:73" x14ac:dyDescent="0.15">
+      <c r="AK27" s="94" t="s">
         <v>173</v>
       </c>
-      <c r="AL26" s="95">
-        <f>AL25/Q19</f>
-        <v>169.35841080663405</v>
-      </c>
-    </row>
-    <row r="27" spans="2:73" x14ac:dyDescent="0.2">
-      <c r="AK27" s="93" t="s">
-        <v>174</v>
-      </c>
-      <c r="AL27" s="40">
+      <c r="AL27" s="97">
         <f>Main!C6</f>
         <v>188.83</v>
       </c>
     </row>
-    <row r="28" spans="2:73" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:73" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
         <v>81</v>
       </c>
@@ -4114,46 +4478,58 @@
       <c r="H28" s="41"/>
       <c r="I28" s="41"/>
       <c r="J28" s="41">
-        <f t="shared" ref="J28:M28" si="46">J9/J5</f>
+        <f t="shared" ref="J28:M28" si="64">J9/J5</f>
         <v>0.62486070575749542</v>
       </c>
       <c r="K28" s="41">
-        <f t="shared" ref="K28" si="47">K9/K5</f>
+        <f t="shared" ref="K28" si="65">K9/K5</f>
         <v>0.63251785723442333</v>
       </c>
       <c r="L28" s="41">
-        <f t="shared" si="46"/>
+        <f t="shared" si="64"/>
         <v>0.63040288854864135</v>
       </c>
       <c r="M28" s="41">
-        <f t="shared" si="46"/>
+        <f t="shared" si="64"/>
         <v>0.62316316721913545</v>
       </c>
       <c r="N28" s="41">
-        <f t="shared" ref="N28:O28" si="48">N9/N5</f>
+        <f t="shared" ref="N28:O28" si="66">N9/N5</f>
         <v>0.62074750204524354</v>
       </c>
       <c r="O28" s="41">
-        <f t="shared" si="48"/>
+        <f t="shared" si="66"/>
         <v>0.60734480902872556</v>
       </c>
       <c r="P28" s="41">
-        <f t="shared" ref="P28:Q28" si="49">P9/P5</f>
+        <f t="shared" ref="P28:Q28" si="67">P9/P5</f>
         <v>0.60908642113629285</v>
       </c>
       <c r="Q28" s="41">
-        <f t="shared" si="49"/>
+        <f t="shared" si="67"/>
         <v>0.61990223060490002</v>
       </c>
-      <c r="R28" s="75">
+      <c r="R28" s="60">
         <v>0.62</v>
       </c>
+      <c r="U28" s="41">
+        <f t="shared" ref="U28:V28" si="68">U9/U5</f>
+        <v>0.61557414513840614</v>
+      </c>
+      <c r="V28" s="41">
+        <f t="shared" ref="V28:X28" si="69">V9/V5</f>
+        <v>0.57884564668650873</v>
+      </c>
+      <c r="W28" s="41">
+        <f t="shared" si="69"/>
+        <v>0.61134972973687329</v>
+      </c>
       <c r="X28" s="41">
-        <f t="shared" ref="X28:Y28" si="50">X9/X5</f>
+        <f t="shared" ref="X28:Y28" si="70">X9/X5</f>
         <v>0.62650208888080705</v>
       </c>
-      <c r="Y28" s="75">
-        <f t="shared" si="50"/>
+      <c r="Y28" s="60">
+        <f t="shared" si="70"/>
         <v>0.61465297760591753</v>
       </c>
       <c r="Z28" s="41">
@@ -4186,40 +4562,40 @@
       <c r="AI28" s="41">
         <v>0.63</v>
       </c>
-      <c r="AK28" s="93" t="s">
-        <v>175</v>
-      </c>
-      <c r="AL28" s="41">
+      <c r="AK28" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="AL28" s="101">
         <f>AL26/AL27-1</f>
-        <v>-0.10311703221609891</v>
-      </c>
-    </row>
-    <row r="29" spans="2:73" x14ac:dyDescent="0.2">
+        <v>-0.12129409881906617</v>
+      </c>
+    </row>
+    <row r="29" spans="2:73" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
         <v>82</v>
       </c>
       <c r="J29" s="41">
-        <f t="shared" ref="J29:M29" si="51">J13/J5</f>
+        <f t="shared" ref="J29:M29" si="71">J13/J5</f>
         <v>2.553727779251791E-2</v>
       </c>
       <c r="K29" s="41">
-        <f t="shared" ref="K29" si="52">K13/K5</f>
+        <f t="shared" ref="K29" si="72">K13/K5</f>
         <v>-0.2577287341233418</v>
       </c>
       <c r="L29" s="41">
-        <f t="shared" si="51"/>
+        <f t="shared" si="71"/>
         <v>-0.42818620169565136</v>
       </c>
       <c r="M29" s="41">
-        <f t="shared" si="51"/>
+        <f t="shared" si="71"/>
         <v>1.2457487208445292E-2</v>
       </c>
       <c r="N29" s="41">
-        <f t="shared" ref="N29:O29" si="53">N13/N5</f>
+        <f t="shared" ref="N29:O29" si="73">N13/N5</f>
         <v>-0.12439676805559401</v>
       </c>
       <c r="O29" s="41">
-        <f t="shared" si="53"/>
+        <f t="shared" si="73"/>
         <v>6.7052482977545028E-2</v>
       </c>
       <c r="P29" s="41">
@@ -4227,88 +4603,100 @@
         <v>7.4965075119129837E-2</v>
       </c>
       <c r="Q29" s="41">
-        <f t="shared" ref="Q29:R29" si="54">Q13/Q5</f>
+        <f t="shared" ref="Q29:R29" si="74">Q13/Q5</f>
         <v>0.10298825355889579</v>
       </c>
-      <c r="R29" s="75">
-        <f t="shared" si="54"/>
-        <v>0.13639999999999997</v>
+      <c r="R29" s="60">
+        <f t="shared" si="74"/>
+        <v>0.13020000000000007</v>
+      </c>
+      <c r="U29" s="41">
+        <f t="shared" ref="U29:V29" si="75">U13/U5</f>
+        <v>5.9135663749678574E-2</v>
+      </c>
+      <c r="V29" s="41">
+        <f t="shared" ref="V29:X29" si="76">V13/V5</f>
+        <v>-1.2044606864333248E-2</v>
+      </c>
+      <c r="W29" s="41">
+        <f t="shared" si="76"/>
+        <v>-2.077817572022457E-2</v>
       </c>
       <c r="X29" s="41">
         <f>X13/X5</f>
         <v>-0.19472631433862925</v>
       </c>
-      <c r="Y29" s="75">
-        <f t="shared" ref="Y29" si="55">Y13/Y5</f>
-        <v>9.8137134127283004E-2</v>
+      <c r="Y29" s="60">
+        <f t="shared" ref="Y29" si="77">Y13/Y5</f>
+        <v>9.6364798323978554E-2</v>
       </c>
       <c r="Z29" s="41">
         <f>Z13/Z5</f>
-        <v>8.8999999999999996E-2</v>
+        <v>2.6999999999999975E-2</v>
       </c>
       <c r="AA29" s="41">
-        <f t="shared" ref="AA29:AI29" si="56">AA13/AA5</f>
+        <f t="shared" ref="AA29:AI29" si="78">AA13/AA5</f>
         <v>2.0500000000000032E-2</v>
       </c>
       <c r="AB29" s="41">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>2.0499999999999952E-2</v>
       </c>
       <c r="AC29" s="41">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>2.0499999999999904E-2</v>
       </c>
       <c r="AD29" s="41">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>2.0500000000000049E-2</v>
       </c>
       <c r="AE29" s="41">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>2.0499999999999977E-2</v>
       </c>
       <c r="AF29" s="41">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>4.0500000000000015E-2</v>
       </c>
       <c r="AG29" s="41">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>4.0500000000000057E-2</v>
       </c>
       <c r="AH29" s="41">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>4.0499999999999994E-2</v>
       </c>
       <c r="AI29" s="41">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>4.0500000000000015E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:73" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:73" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
         <v>83</v>
       </c>
       <c r="J30" s="41">
-        <f t="shared" ref="J30:M30" si="57">J17/J5</f>
+        <f t="shared" ref="J30:M30" si="79">J17/J5</f>
         <v>0.11423896701158574</v>
       </c>
       <c r="K30" s="41">
-        <f t="shared" ref="K30" si="58">K17/K5</f>
+        <f t="shared" ref="K30" si="80">K17/K5</f>
         <v>-0.24570426471266901</v>
       </c>
       <c r="L30" s="41">
-        <f t="shared" si="57"/>
+        <f t="shared" si="79"/>
         <v>-0.21534769990173466</v>
       </c>
       <c r="M30" s="41">
-        <f t="shared" si="57"/>
+        <f t="shared" si="79"/>
         <v>0.20916508972408179</v>
       </c>
       <c r="N30" s="41">
-        <f t="shared" ref="N30:O30" si="59">N17/N5</f>
+        <f t="shared" ref="N30:O30" si="81">N17/N5</f>
         <v>-6.2083482705053032E-2</v>
       </c>
       <c r="O30" s="41">
-        <f t="shared" si="59"/>
+        <f t="shared" si="81"/>
         <v>0.21382777097486202</v>
       </c>
       <c r="P30" s="41">
@@ -4316,88 +4704,100 @@
         <v>0.17843025352487471</v>
       </c>
       <c r="Q30" s="41">
-        <f t="shared" ref="Q30:R30" si="60">Q17/Q5</f>
+        <f t="shared" ref="Q30:R30" si="82">Q17/Q5</f>
         <v>3.8912090943500309E-2</v>
       </c>
-      <c r="R30" s="75">
-        <f t="shared" si="60"/>
-        <v>0.13967507097954565</v>
+      <c r="R30" s="60">
+        <f t="shared" si="82"/>
+        <v>0.13601707097954571</v>
+      </c>
+      <c r="U30" s="41">
+        <f t="shared" ref="U30:V30" si="83">U17/U5</f>
+        <v>6.9524457944904111E-2</v>
+      </c>
+      <c r="V30" s="41">
+        <f t="shared" ref="V30:X30" si="84">V17/V5</f>
+        <v>1.661454997551241E-3</v>
+      </c>
+      <c r="W30" s="41">
+        <f t="shared" si="84"/>
+        <v>-2.5315600665490328E-3</v>
       </c>
       <c r="X30" s="41">
         <f>X17/X5</f>
         <v>-6.9515080827583717E-2</v>
       </c>
-      <c r="Y30" s="75">
-        <f t="shared" ref="Y30" si="61">Y17/Y5</f>
-        <v>0.13856295339115768</v>
+      <c r="Y30" s="60">
+        <f t="shared" ref="Y30" si="85">Y17/Y5</f>
+        <v>0.13751727526720806</v>
       </c>
       <c r="Z30" s="41">
         <f>Z17/Z5</f>
-        <v>7.8144512466667843E-2</v>
+        <v>4.0262103925556708E-2</v>
       </c>
       <c r="AA30" s="41">
-        <f t="shared" ref="AA30:AI30" si="62">AA17/AA5</f>
-        <v>3.3618180739180201E-2</v>
+        <f t="shared" ref="AA30:AI30" si="86">AA17/AA5</f>
+        <v>3.4207973383727226E-2</v>
       </c>
       <c r="AB30" s="41">
-        <f t="shared" si="62"/>
+        <f t="shared" si="86"/>
         <v>2.5715470982967552E-2</v>
       </c>
       <c r="AC30" s="41">
-        <f t="shared" si="62"/>
-        <v>2.1890482532147561E-2</v>
+        <f t="shared" si="86"/>
+        <v>2.0696456212212239E-2</v>
       </c>
       <c r="AD30" s="41">
-        <f t="shared" si="62"/>
-        <v>1.8837508109649622E-2</v>
+        <f t="shared" si="86"/>
+        <v>1.7810007667305096E-2</v>
       </c>
       <c r="AE30" s="41">
-        <f t="shared" si="62"/>
-        <v>1.6966855545008448E-2</v>
+        <f t="shared" si="86"/>
+        <v>1.3573484436006754E-2</v>
       </c>
       <c r="AF30" s="41">
-        <f t="shared" si="62"/>
-        <v>2.6457856816299322E-2</v>
+        <f t="shared" si="86"/>
+        <v>2.0685233510924925E-2</v>
       </c>
       <c r="AG30" s="41">
-        <f t="shared" si="62"/>
-        <v>2.5385757818110467E-2</v>
+        <f t="shared" si="86"/>
+        <v>1.9385487788375264E-2</v>
       </c>
       <c r="AH30" s="41">
-        <f t="shared" si="62"/>
-        <v>2.4574692694306829E-2</v>
+        <f t="shared" si="86"/>
+        <v>1.8319316372119636E-2</v>
       </c>
       <c r="AI30" s="41">
-        <f t="shared" si="62"/>
+        <f t="shared" si="86"/>
         <v>2.3980169535095935E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:73" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:73" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>84</v>
       </c>
       <c r="J31" s="41">
-        <f t="shared" ref="J31:M31" si="63">J16/J15</f>
+        <f t="shared" ref="J31:M31" si="87">J16/J15</f>
         <v>-1.8577433628318583</v>
       </c>
       <c r="K31" s="41">
-        <f t="shared" ref="K31" si="64">K16/K15</f>
+        <f t="shared" ref="K31" si="88">K16/K15</f>
         <v>3.5428870503452302E-2</v>
       </c>
       <c r="L31" s="41">
-        <f t="shared" si="63"/>
+        <f t="shared" si="87"/>
         <v>9.1177378288712238E-2</v>
       </c>
       <c r="M31" s="41">
-        <f t="shared" si="63"/>
+        <f t="shared" si="87"/>
         <v>19.380303030303139</v>
       </c>
       <c r="N31" s="41">
-        <f t="shared" ref="N31:O31" si="65">N16/N15</f>
+        <f t="shared" ref="N31:O31" si="89">N16/N15</f>
         <v>0.63701832643628697</v>
       </c>
       <c r="O31" s="41">
-        <f t="shared" si="65"/>
+        <f t="shared" si="89"/>
         <v>0.24363731670644073</v>
       </c>
       <c r="P31" s="41">
@@ -4405,84 +4805,99 @@
         <v>0.2553443312827855</v>
       </c>
       <c r="Q31" s="41">
-        <f t="shared" ref="Q31:R31" si="66">Q16/Q15</f>
+        <f t="shared" ref="Q31" si="90">Q16/Q15</f>
         <v>0.41840061367341075</v>
       </c>
-      <c r="R31" s="75">
+      <c r="R31" s="60">
         <v>0.41</v>
+      </c>
+      <c r="U31" s="41">
+        <f t="shared" ref="U31:V31" si="91">U16/U15</f>
+        <v>-3.9175918018787392E-2</v>
+      </c>
+      <c r="V31" s="41">
+        <f t="shared" ref="V31:X31" si="92">V16/V15</f>
+        <v>0.57391304347824645</v>
+      </c>
+      <c r="W31" s="41">
+        <f t="shared" si="92"/>
+        <v>0.72595771737401593</v>
       </c>
       <c r="X31" s="41">
         <f>X16/X15</f>
         <v>0.57546949602121988</v>
       </c>
-      <c r="Y31" s="75">
+      <c r="Y31" s="60">
         <v>0.41</v>
       </c>
       <c r="Z31" s="41">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="AA31" s="41">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="AB31" s="41">
         <v>0.43</v>
       </c>
       <c r="AC31" s="41">
-        <v>0.45</v>
+        <v>0.48</v>
       </c>
       <c r="AD31" s="41">
-        <v>0.45</v>
+        <v>0.48</v>
       </c>
       <c r="AE31" s="41">
-        <v>0.45</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="AF31" s="41">
-        <v>0.45</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="AG31" s="41">
-        <v>0.45</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="AH31" s="41">
-        <v>0.45</v>
+        <v>0.59</v>
       </c>
       <c r="AI31" s="41">
         <v>0.45</v>
       </c>
     </row>
-    <row r="32" spans="2:73" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:73" x14ac:dyDescent="0.15">
       <c r="K32" s="41"/>
       <c r="L32" s="41"/>
       <c r="O32" s="41"/>
       <c r="P32" s="41"/>
       <c r="Q32" s="41"/>
+      <c r="U32" s="41"/>
+      <c r="V32" s="41"/>
+      <c r="W32" s="41"/>
       <c r="X32" s="41"/>
     </row>
-    <row r="33" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
         <v>150</v>
       </c>
       <c r="J33" s="41">
-        <f t="shared" ref="J33:O33" si="67">J11/J5</f>
+        <f t="shared" ref="J33:O33" si="93">J11/J5</f>
         <v>0.16807287521004688</v>
       </c>
       <c r="K33" s="41">
-        <f t="shared" ref="K33" si="68">K11/K5</f>
+        <f t="shared" ref="K33" si="94">K11/K5</f>
         <v>0.24109445746311897</v>
       </c>
       <c r="L33" s="41">
-        <f t="shared" si="67"/>
+        <f t="shared" si="93"/>
         <v>0.24658698781964852</v>
       </c>
       <c r="M33" s="41">
-        <f t="shared" si="67"/>
+        <f t="shared" si="93"/>
         <v>0.18268969649423031</v>
       </c>
       <c r="N33" s="41">
-        <f t="shared" si="67"/>
+        <f t="shared" si="93"/>
         <v>0.23290038514923386</v>
       </c>
       <c r="O33" s="41">
-        <f t="shared" si="67"/>
+        <f t="shared" si="93"/>
         <v>0.1888108070164492</v>
       </c>
       <c r="P33" s="41">
@@ -4490,19 +4905,31 @@
         <v>0.20148592676103677</v>
       </c>
       <c r="Q33" s="41">
-        <f t="shared" ref="Q33" si="69">Q11/Q5</f>
+        <f t="shared" ref="Q33" si="95">Q11/Q5</f>
         <v>0.18965915433322428</v>
       </c>
-      <c r="R33" s="75">
-        <v>0.2</v>
+      <c r="R33" s="60">
+        <v>0.21</v>
+      </c>
+      <c r="U33" s="41">
+        <f t="shared" ref="U33:V33" si="96">U11/U5</f>
+        <v>0.18296085395697839</v>
+      </c>
+      <c r="V33" s="41">
+        <f t="shared" ref="V33:X33" si="97">V11/V5</f>
+        <v>0.18973175601853595</v>
+      </c>
+      <c r="W33" s="41">
+        <f t="shared" si="97"/>
+        <v>0.18090228677406708</v>
       </c>
       <c r="X33" s="41">
         <f>X11/X5</f>
         <v>0.22472813277104781</v>
       </c>
-      <c r="Y33" s="75">
+      <c r="Y33" s="60">
         <f>Y11/Y5</f>
-        <v>0.1735331975994549</v>
+        <v>0.17530553340275937</v>
       </c>
       <c r="Z33" s="41">
         <v>0.19</v>
@@ -4535,12 +4962,12 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="34" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:35" x14ac:dyDescent="0.15">
       <c r="L34" s="41"/>
       <c r="O34" s="41"/>
       <c r="P34" s="41"/>
     </row>
-    <row r="35" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B35" s="50" t="s">
         <v>103</v>
       </c>
@@ -4548,7 +4975,7 @@
       <c r="O35" s="41"/>
       <c r="P35" s="41"/>
     </row>
-    <row r="36" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
         <v>36</v>
       </c>
@@ -4578,11 +5005,11 @@
       <c r="P36" s="40">
         <v>32.79</v>
       </c>
-      <c r="Q36" s="79">
+      <c r="Q36" s="64">
         <v>40.502000000000002</v>
       </c>
     </row>
-    <row r="37" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
@@ -4612,11 +5039,11 @@
       <c r="P37" s="40">
         <v>8.8309999999999995</v>
       </c>
-      <c r="Q37" s="79">
+      <c r="Q37" s="64">
         <v>6.9560000000000004</v>
       </c>
     </row>
-    <row r="38" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
@@ -4646,11 +5073,11 @@
       <c r="P38" s="40">
         <v>2.7450000000000001</v>
       </c>
-      <c r="Q38" s="79">
+      <c r="Q38" s="64">
         <v>5.12</v>
       </c>
     </row>
-    <row r="39" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
@@ -4680,11 +5107,11 @@
       <c r="P39" s="40">
         <v>5.157</v>
       </c>
-      <c r="Q39" s="79">
+      <c r="Q39" s="64">
         <v>7.18</v>
       </c>
     </row>
-    <row r="40" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>98</v>
       </c>
@@ -4714,11 +5141,11 @@
       <c r="P40" s="40">
         <v>1536.3320000000001</v>
       </c>
-      <c r="Q40" s="79">
+      <c r="Q40" s="64">
         <v>1327.1690000000001</v>
       </c>
     </row>
-    <row r="41" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
         <v>99</v>
       </c>
@@ -4748,11 +5175,11 @@
       <c r="P41" s="40">
         <v>59.850999999999999</v>
       </c>
-      <c r="Q41" s="79">
+      <c r="Q41" s="64">
         <v>71.069999999999993</v>
       </c>
     </row>
-    <row r="42" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>100</v>
       </c>
@@ -4782,11 +5209,11 @@
       <c r="P42" s="40">
         <v>1.1359999999999999</v>
       </c>
-      <c r="Q42" s="79">
+      <c r="Q42" s="64">
         <v>1.1879999999999999</v>
       </c>
     </row>
-    <row r="43" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>101</v>
       </c>
@@ -4816,11 +5243,11 @@
       <c r="P43" s="40">
         <v>6.1459999999999999</v>
       </c>
-      <c r="Q43" s="79">
+      <c r="Q43" s="64">
         <v>2.3420000000000001</v>
       </c>
     </row>
-    <row r="44" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>102</v>
       </c>
@@ -4850,21 +5277,21 @@
       <c r="P44" s="40">
         <v>5.3140000000000001</v>
       </c>
-      <c r="Q44" s="79">
+      <c r="Q44" s="64">
         <v>3.8220000000000001</v>
       </c>
     </row>
-    <row r="45" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:35" x14ac:dyDescent="0.15">
       <c r="L45" s="41"/>
       <c r="O45" s="41"/>
       <c r="P45" s="41"/>
     </row>
-    <row r="47" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B47" s="45" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B48" s="2" t="s">
         <v>5</v>
       </c>
@@ -4880,13 +5307,13 @@
       <c r="P48" s="39">
         <v>212.815</v>
       </c>
-      <c r="Q48" s="78">
+      <c r="Q48" s="63">
         <v>147.71100000000001</v>
       </c>
-      <c r="R48" s="85"/>
-      <c r="Y48" s="85"/>
-    </row>
-    <row r="49" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R48" s="70"/>
+      <c r="Y48" s="70"/>
+    </row>
+    <row r="49" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B49" s="2" t="s">
         <v>104</v>
       </c>
@@ -4902,13 +5329,13 @@
       <c r="P49" s="39">
         <v>45.9</v>
       </c>
-      <c r="Q49" s="78">
+      <c r="Q49" s="63">
         <v>35.28</v>
       </c>
-      <c r="R49" s="85"/>
-      <c r="Y49" s="85"/>
-    </row>
-    <row r="50" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R49" s="70"/>
+      <c r="Y49" s="70"/>
+    </row>
+    <row r="50" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B50" s="2" t="s">
         <v>105</v>
       </c>
@@ -4924,13 +5351,13 @@
       <c r="P50" s="39">
         <v>118.514</v>
       </c>
-      <c r="Q50" s="78">
+      <c r="Q50" s="63">
         <v>194.62700000000001</v>
       </c>
-      <c r="R50" s="85"/>
-      <c r="Y50" s="85"/>
-    </row>
-    <row r="51" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="R50" s="70"/>
+      <c r="Y50" s="70"/>
+    </row>
+    <row r="51" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
         <v>106</v>
       </c>
@@ -4946,11 +5373,11 @@
       <c r="P51" s="40">
         <v>379.67200000000003</v>
       </c>
-      <c r="Q51" s="79">
+      <c r="Q51" s="64">
         <v>418.30799999999999</v>
       </c>
     </row>
-    <row r="52" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
         <v>107</v>
       </c>
@@ -4966,11 +5393,11 @@
       <c r="P52" s="40">
         <v>196.75399999999999</v>
       </c>
-      <c r="Q52" s="79">
+      <c r="Q52" s="64">
         <v>168.673</v>
       </c>
     </row>
-    <row r="53" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B53" s="2" t="s">
         <v>108</v>
       </c>
@@ -4986,13 +5413,13 @@
       <c r="P53" s="39">
         <v>154.297</v>
       </c>
-      <c r="Q53" s="78">
+      <c r="Q53" s="63">
         <v>173.04599999999999</v>
       </c>
-      <c r="R53" s="85"/>
-      <c r="Y53" s="85"/>
-    </row>
-    <row r="54" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="R53" s="70"/>
+      <c r="Y53" s="70"/>
+    </row>
+    <row r="54" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
         <v>109</v>
       </c>
@@ -5008,11 +5435,11 @@
       <c r="P54" s="40">
         <v>61.838999999999999</v>
       </c>
-      <c r="Q54" s="79">
+      <c r="Q54" s="64">
         <v>68.055999999999997</v>
       </c>
     </row>
-    <row r="55" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B55" s="1" t="s">
         <v>110</v>
       </c>
@@ -5037,7 +5464,7 @@
         <v>1205.701</v>
       </c>
     </row>
-    <row r="56" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
         <v>111</v>
       </c>
@@ -5053,11 +5480,11 @@
       <c r="P56" s="40">
         <v>157.916</v>
       </c>
-      <c r="Q56" s="79">
+      <c r="Q56" s="64">
         <v>164.16</v>
       </c>
     </row>
-    <row r="57" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B57" s="1" t="s">
         <v>112</v>
       </c>
@@ -5073,11 +5500,11 @@
       <c r="P57" s="40">
         <v>100.548</v>
       </c>
-      <c r="Q57" s="79">
+      <c r="Q57" s="64">
         <v>96.355000000000004</v>
       </c>
     </row>
-    <row r="58" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B58" s="1" t="s">
         <v>113</v>
       </c>
@@ -5097,12 +5524,12 @@
         <f>13.934+45.004</f>
         <v>58.937999999999995</v>
       </c>
-      <c r="Q58" s="79">
+      <c r="Q58" s="64">
         <f>13.039+44.819</f>
         <v>57.858000000000004</v>
       </c>
     </row>
-    <row r="59" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B59" s="2" t="s">
         <v>114</v>
       </c>
@@ -5118,13 +5545,13 @@
       <c r="P59" s="39">
         <v>24.925000000000001</v>
       </c>
-      <c r="Q59" s="78">
+      <c r="Q59" s="63">
         <v>28.536000000000001</v>
       </c>
-      <c r="R59" s="85"/>
-      <c r="Y59" s="85"/>
-    </row>
-    <row r="60" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="R59" s="70"/>
+      <c r="Y59" s="70"/>
+    </row>
+    <row r="60" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
         <v>115</v>
       </c>
@@ -5140,11 +5567,11 @@
       <c r="P60" s="40">
         <v>8.9920000000000009</v>
       </c>
-      <c r="Q60" s="79">
+      <c r="Q60" s="64">
         <v>8.4619999999999997</v>
       </c>
     </row>
-    <row r="61" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B61" s="1" t="s">
         <v>116</v>
       </c>
@@ -5160,11 +5587,11 @@
       <c r="P61" s="40">
         <v>28.24</v>
       </c>
-      <c r="Q61" s="79">
+      <c r="Q61" s="64">
         <v>48.387999999999998</v>
       </c>
     </row>
-    <row r="62" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
         <v>117</v>
       </c>
@@ -5180,11 +5607,11 @@
       <c r="P62" s="40">
         <v>281.69099999999997</v>
       </c>
-      <c r="Q62" s="79">
+      <c r="Q62" s="64">
         <v>290.32900000000001</v>
       </c>
     </row>
-    <row r="63" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B63" s="1" t="s">
         <v>118</v>
       </c>
@@ -5200,11 +5627,11 @@
       <c r="P63" s="40">
         <v>100.982</v>
       </c>
-      <c r="Q63" s="79">
+      <c r="Q63" s="64">
         <v>110.643</v>
       </c>
     </row>
-    <row r="64" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B64" s="1" t="s">
         <v>119</v>
       </c>
@@ -5229,13 +5656,13 @@
         <v>2010.432</v>
       </c>
     </row>
-    <row r="65" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:25" x14ac:dyDescent="0.15">
       <c r="K65" s="40"/>
       <c r="N65" s="40"/>
       <c r="P65" s="52"/>
-      <c r="Q65" s="79"/>
-    </row>
-    <row r="66" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="Q65" s="64"/>
+    </row>
+    <row r="66" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B66" s="1" t="s">
         <v>120</v>
       </c>
@@ -5251,11 +5678,11 @@
       <c r="P66" s="52">
         <v>60.689</v>
       </c>
-      <c r="Q66" s="79">
+      <c r="Q66" s="64">
         <v>50.192999999999998</v>
       </c>
     </row>
-    <row r="67" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B67" s="1" t="s">
         <v>121</v>
       </c>
@@ -5271,11 +5698,11 @@
       <c r="P67" s="52">
         <v>100.98</v>
       </c>
-      <c r="Q67" s="79">
+      <c r="Q67" s="64">
         <v>112.76600000000001</v>
       </c>
     </row>
-    <row r="68" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B68" s="1" t="s">
         <v>125</v>
       </c>
@@ -5291,11 +5718,11 @@
       <c r="P68" s="52">
         <v>253.185</v>
       </c>
-      <c r="Q68" s="79">
+      <c r="Q68" s="64">
         <v>246.46600000000001</v>
       </c>
     </row>
-    <row r="69" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B69" s="2" t="s">
         <v>122</v>
       </c>
@@ -5311,13 +5738,13 @@
       <c r="P69" s="51">
         <v>11.33</v>
       </c>
-      <c r="Q69" s="78">
+      <c r="Q69" s="63">
         <v>15.317</v>
       </c>
-      <c r="R69" s="85"/>
-      <c r="Y69" s="85"/>
-    </row>
-    <row r="70" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="R69" s="70"/>
+      <c r="Y69" s="70"/>
+    </row>
+    <row r="70" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B70" s="1" t="s">
         <v>123</v>
       </c>
@@ -5333,11 +5760,11 @@
       <c r="P70" s="52">
         <v>6.7869999999999999</v>
       </c>
-      <c r="Q70" s="79">
+      <c r="Q70" s="64">
         <v>6.8010000000000002</v>
       </c>
     </row>
-    <row r="71" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B71" s="1" t="s">
         <v>124</v>
       </c>
@@ -5362,7 +5789,7 @@
         <v>431.54300000000001</v>
       </c>
     </row>
-    <row r="72" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B72" s="1" t="s">
         <v>126</v>
       </c>
@@ -5378,11 +5805,11 @@
       <c r="P72" s="52">
         <v>269.47699999999998</v>
       </c>
-      <c r="Q72" s="79">
+      <c r="Q72" s="64">
         <v>313.82299999999998</v>
       </c>
     </row>
-    <row r="73" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B73" s="1" t="s">
         <v>127</v>
       </c>
@@ -5398,11 +5825,11 @@
       <c r="P73" s="52">
         <v>7.6920000000000002</v>
       </c>
-      <c r="Q73" s="79">
+      <c r="Q73" s="64">
         <v>7.3170000000000002</v>
       </c>
     </row>
-    <row r="74" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B74" s="1" t="s">
         <v>137</v>
       </c>
@@ -5418,11 +5845,11 @@
       <c r="P74" s="52">
         <v>5.5170000000000003</v>
       </c>
-      <c r="Q74" s="79">
+      <c r="Q74" s="64">
         <v>5.3689999999999998</v>
       </c>
     </row>
-    <row r="75" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B75" s="1" t="s">
         <v>140</v>
       </c>
@@ -5438,11 +5865,11 @@
       <c r="P75" s="52">
         <v>1E-3</v>
       </c>
-      <c r="Q75" s="79">
+      <c r="Q75" s="64">
         <v>0.01</v>
       </c>
     </row>
-    <row r="76" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B76" s="1" t="s">
         <v>128</v>
       </c>
@@ -5458,11 +5885,11 @@
       <c r="P76" s="52">
         <v>18.21</v>
       </c>
-      <c r="Q76" s="79">
+      <c r="Q76" s="64">
         <v>16.311</v>
       </c>
     </row>
-    <row r="77" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B77" s="1" t="s">
         <v>129</v>
       </c>
@@ -5478,11 +5905,11 @@
       <c r="P77" s="52">
         <v>4.5039999999999996</v>
       </c>
-      <c r="Q77" s="79">
+      <c r="Q77" s="64">
         <v>4.7729999999999997</v>
       </c>
     </row>
-    <row r="78" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B78" s="1" t="s">
         <v>130</v>
       </c>
@@ -5507,10 +5934,10 @@
         <v>779.14599999999996</v>
       </c>
     </row>
-    <row r="79" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:25" x14ac:dyDescent="0.15">
       <c r="N79" s="40"/>
     </row>
-    <row r="80" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B80" s="1" t="s">
         <v>131</v>
       </c>
@@ -5526,11 +5953,11 @@
       <c r="P80" s="40">
         <v>1193.6510000000001</v>
       </c>
-      <c r="Q80" s="79">
+      <c r="Q80" s="64">
         <v>1231.3130000000001</v>
       </c>
     </row>
-    <row r="81" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B81" s="1" t="s">
         <v>132</v>
       </c>
@@ -5555,10 +5982,10 @@
         <v>2010.4590000000001</v>
       </c>
     </row>
-    <row r="82" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:25" x14ac:dyDescent="0.15">
       <c r="N82" s="40"/>
     </row>
-    <row r="83" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B83" s="1" t="s">
         <v>133</v>
       </c>
@@ -5579,11 +6006,11 @@
         <v>1193.6509999999998</v>
       </c>
       <c r="Q83" s="40">
-        <f t="shared" ref="Q83" si="70">Q64-Q78</f>
+        <f t="shared" ref="Q83" si="98">Q64-Q78</f>
         <v>1231.2860000000001</v>
       </c>
     </row>
-    <row r="84" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B84" s="1" t="s">
         <v>134</v>
       </c>
@@ -5604,16 +6031,16 @@
         <v>16.802519707207203</v>
       </c>
       <c r="Q84" s="40">
-        <f t="shared" ref="Q84" si="71">Q83/Q19</f>
+        <f t="shared" ref="Q84" si="99">Q83/Q19</f>
         <v>17.315960453963747</v>
       </c>
     </row>
-    <row r="86" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B86" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="87" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B87" s="2" t="s">
         <v>136</v>
       </c>
@@ -5625,11 +6052,11 @@
         <f>N53/J53-1</f>
         <v>0.20820827497276517</v>
       </c>
-      <c r="Q87" s="81"/>
-      <c r="R87" s="85"/>
-      <c r="Y87" s="85"/>
-    </row>
-    <row r="89" spans="2:25" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q87" s="66"/>
+      <c r="R87" s="70"/>
+      <c r="Y87" s="70"/>
+    </row>
+    <row r="89" spans="2:25" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B89" s="35" t="s">
         <v>5</v>
       </c>
@@ -5638,7 +6065,7 @@
         <v>561.96499999999992</v>
       </c>
       <c r="K89" s="38">
-        <f t="shared" ref="K89" si="72">K48+K49+K50</f>
+        <f t="shared" ref="K89" si="100">K48+K49+K50</f>
         <v>595.72399999999993</v>
       </c>
       <c r="N89" s="38">
@@ -5650,13 +6077,13 @@
         <v>377.22899999999998</v>
       </c>
       <c r="Q89" s="38">
-        <f t="shared" ref="Q89" si="73">Q48+Q49+Q50</f>
+        <f t="shared" ref="Q89" si="101">Q48+Q49+Q50</f>
         <v>377.61800000000005</v>
       </c>
       <c r="R89" s="48"/>
       <c r="Y89" s="48"/>
     </row>
-    <row r="90" spans="2:25" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:25" s="35" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B90" s="35" t="s">
         <v>6</v>
       </c>
@@ -5678,7 +6105,7 @@
       <c r="R90" s="48"/>
       <c r="Y90" s="48"/>
     </row>
-    <row r="91" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B91" s="1" t="s">
         <v>7</v>
       </c>
@@ -5687,7 +6114,7 @@
         <v>561.96499999999992</v>
       </c>
       <c r="K91" s="40">
-        <f t="shared" ref="K91" si="74">K89-K90</f>
+        <f t="shared" ref="K91" si="102">K89-K90</f>
         <v>595.72399999999993</v>
       </c>
       <c r="N91" s="40">
@@ -5699,11 +6126,11 @@
         <v>377.22899999999998</v>
       </c>
       <c r="Q91" s="40">
-        <f t="shared" ref="Q91" si="75">Q89-Q90</f>
+        <f t="shared" ref="Q91" si="103">Q89-Q90</f>
         <v>377.61800000000005</v>
       </c>
     </row>
-    <row r="93" spans="2:25" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:25" s="43" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B93" s="43" t="s">
         <v>138</v>
       </c>
@@ -5728,38 +6155,38 @@
       <c r="P93" s="43">
         <v>93.17</v>
       </c>
-      <c r="Q93" s="83">
+      <c r="Q93" s="68">
         <v>115.75</v>
       </c>
-      <c r="R93" s="86"/>
-      <c r="Y93" s="86"/>
-    </row>
-    <row r="94" spans="2:25" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R93" s="71"/>
+      <c r="Y93" s="71"/>
+    </row>
+    <row r="94" spans="2:25" s="40" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B94" s="40" t="s">
         <v>139</v>
       </c>
       <c r="J94" s="40">
-        <f t="shared" ref="J94:O94" si="76">J93*J19</f>
+        <f t="shared" ref="J94:O94" si="104">J93*J19</f>
         <v>7797.68667</v>
       </c>
       <c r="K94" s="40">
-        <f t="shared" ref="K94" si="77">K93*K19</f>
+        <f t="shared" ref="K94" si="105">K93*K19</f>
         <v>9120.0071200000002</v>
       </c>
       <c r="L94" s="40">
-        <f t="shared" si="76"/>
+        <f t="shared" si="104"/>
         <v>11521.3488</v>
       </c>
       <c r="M94" s="40">
-        <f t="shared" si="76"/>
+        <f t="shared" si="104"/>
         <v>11584.923839999999</v>
       </c>
       <c r="N94" s="40">
-        <f t="shared" si="76"/>
+        <f t="shared" si="104"/>
         <v>10881.67</v>
       </c>
       <c r="O94" s="40">
-        <f t="shared" si="76"/>
+        <f t="shared" si="104"/>
         <v>9771.9434999999994</v>
       </c>
       <c r="P94" s="40">
@@ -5767,13 +6194,13 @@
         <v>6618.796800000001</v>
       </c>
       <c r="Q94" s="40">
-        <f t="shared" ref="Q94" si="78">Q93*Q19</f>
+        <f t="shared" ref="Q94" si="106">Q93*Q19</f>
         <v>8230.6352499999994</v>
       </c>
       <c r="R94" s="47"/>
       <c r="Y94" s="47"/>
     </row>
-    <row r="95" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B95" s="1" t="s">
         <v>8</v>
       </c>
@@ -5782,7 +6209,7 @@
         <v>7235.7216699999999</v>
       </c>
       <c r="K95" s="40">
-        <f t="shared" ref="K95" si="79">K94-K91</f>
+        <f t="shared" ref="K95" si="107">K94-K91</f>
         <v>8524.2831200000001</v>
       </c>
       <c r="N95" s="40">
@@ -5794,11 +6221,11 @@
         <v>6241.5678000000007</v>
       </c>
       <c r="Q95" s="40">
-        <f t="shared" ref="Q95" si="80">Q94-Q91</f>
+        <f t="shared" ref="Q95" si="108">Q94-Q91</f>
         <v>7853.017249999999</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A97" s="59">
         <f>AVERAGE(C97:AG97)</f>
         <v>10.162747205497784</v>
@@ -5807,15 +6234,15 @@
         <v>22</v>
       </c>
       <c r="M97" s="56">
-        <f t="shared" ref="M97:O97" si="81">M94/SUM(J5:M5)</f>
+        <f t="shared" ref="M97:O97" si="109">M94/SUM(J5:M5)</f>
         <v>13.2863316065385</v>
       </c>
       <c r="N97" s="56">
-        <f t="shared" si="81"/>
+        <f t="shared" si="109"/>
         <v>12.603555093290217</v>
       </c>
       <c r="O97" s="56">
-        <f t="shared" si="81"/>
+        <f t="shared" si="109"/>
         <v>10.566685013213839</v>
       </c>
       <c r="P97" s="56">
@@ -5823,11 +6250,11 @@
         <v>6.6748252834291053</v>
       </c>
       <c r="Q97" s="56">
-        <f t="shared" ref="Q97" si="82">Q94/SUM(N5:Q5)</f>
+        <f t="shared" ref="Q97" si="110">Q94/SUM(N5:Q5)</f>
         <v>7.682339031017265</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A98" s="59">
         <f>AVERAGE(C98:AG98)</f>
         <v>62.447808359934214</v>
@@ -5847,7 +6274,7 @@
         <v>78.962167745508339</v>
       </c>
     </row>
-    <row r="99" spans="1:25" s="56" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:25" s="56" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A99" s="59">
         <f>AVERAGE(C99:AG99)</f>
         <v>7.925631151755125</v>
@@ -5860,7 +6287,7 @@
         <v>7.9873462056532354</v>
       </c>
       <c r="K99" s="56">
-        <f t="shared" ref="K99" si="83">K93/K84</f>
+        <f t="shared" ref="K99" si="111">K93/K84</f>
         <v>9.021099781990257</v>
       </c>
       <c r="N99" s="56">
@@ -5872,11 +6299,11 @@
         <v>5.545001679720456</v>
       </c>
       <c r="Q99" s="56">
-        <f t="shared" ref="Q99" si="84">Q93/Q84</f>
+        <f t="shared" ref="Q99" si="112">Q93/Q84</f>
         <v>6.6845844507287495</v>
       </c>
-      <c r="R99" s="87"/>
-      <c r="Y99" s="87"/>
+      <c r="R99" s="72"/>
+      <c r="Y99" s="72"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5885,14 +6312,13 @@
     <hyperlink ref="K1" r:id="rId3" xr:uid="{DF1C6BB7-7CFF-5D44-9BEE-5CB961E150F1}"/>
     <hyperlink ref="X1" r:id="rId4" xr:uid="{24C18D69-9B16-5F49-888B-0E1F34CAFFCF}"/>
     <hyperlink ref="Q1" r:id="rId5" xr:uid="{1E775E75-414E-4EF3-BED5-DF18BB35E228}"/>
+    <hyperlink ref="W1" r:id="rId6" xr:uid="{0155C928-42DB-9C49-916E-988EB162F485}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId7"/>
   <ignoredErrors>
-    <ignoredError sqref="X3:X4 X16 X6:X14 R14" formulaRange="1"/>
-    <ignoredError sqref="X15 X5" formula="1" formulaRange="1"/>
-    <ignoredError sqref="Y5 Y9 R16 Y15" formula="1"/>
+    <ignoredError sqref="X3:X4 X16 X6:X7 R14 X10:X11 X14" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>